<commit_message>
scan by barcode log fixing
</commit_message>
<xml_diff>
--- a/Import vender data new.xlsx
+++ b/Import vender data new.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="267">
   <si>
     <t>A</t>
   </si>
@@ -1252,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G16"/>
     </sheetView>
   </sheetViews>
@@ -1672,6 +1673,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="16.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -1721,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F204"/>
   <sheetViews>
@@ -5823,7 +5908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
@@ -6930,7 +7015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F10:I15"/>
   <sheetViews>
@@ -7011,7 +7096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>